<commit_message>
experiment apps for LoRaGW
</commit_message>
<xml_diff>
--- a/project plan.xlsx
+++ b/project plan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Desktop\AI_Lora_Mobility\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\augus\Desktop\Main folder\University\Master\MscThesis\Project\Git\AI_Lora_Mobility\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{031D8020-379E-4912-8F5D-72816A0F6AB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B33AE119-DE70-421E-A8E2-7B04D6075433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project schedule" sheetId="11" r:id="rId1"/>
@@ -18,12 +18,12 @@
   </sheets>
   <definedNames>
     <definedName name="Display_Week">'Project schedule'!$Q$2</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Project schedule'!$4:$6</definedName>
     <definedName name="Project_Start">'Project schedule'!$Q$1</definedName>
     <definedName name="task_end" localSheetId="0">'Project schedule'!$F1</definedName>
     <definedName name="task_progress" localSheetId="0">'Project schedule'!$D1</definedName>
     <definedName name="task_start" localSheetId="0">'Project schedule'!$E1</definedName>
     <definedName name="today" localSheetId="0">TODAY()</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Project schedule'!$4:$6</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="50">
   <si>
     <t>Insert new rows ABOVE this one</t>
   </si>
@@ -156,9 +156,6 @@
   </si>
   <si>
     <t>Setup simulator environment</t>
-  </si>
-  <si>
-    <t>Design simulator environments</t>
   </si>
   <si>
     <t>Idenitfy experiment cases</t>
@@ -1088,19 +1085,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="167" fontId="19" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="19" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="19" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1112,32 +1112,29 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="167" fontId="19" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="19" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="19" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
+    <cellStyle name="Comma" xfId="4" builtinId="3" customBuiltin="1"/>
     <cellStyle name="Date" xfId="10" xr:uid="{229918B6-DD13-4F5A-97B9-305F7E002AA3}"/>
-    <cellStyle name="Komma" xfId="4" builtinId="3" customBuiltin="1"/>
-    <cellStyle name="Link" xfId="1" builtinId="8" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="6" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="7" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="8" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" customBuiltin="1"/>
     <cellStyle name="Name" xfId="11" xr:uid="{B2D3C1EE-6B41-4801-AAFC-C2274E49E503}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Overskrift 1" xfId="6" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Overskrift 2" xfId="7" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Overskrift 3" xfId="8" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Procent" xfId="2" builtinId="5"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
     <cellStyle name="Project Start" xfId="9" xr:uid="{8EB8A09A-C31C-40A3-B2C1-9449520178B8}"/>
     <cellStyle name="Task" xfId="12" xr:uid="{6391D789-272B-4DD2-9BF3-2CDCF610FA41}"/>
-    <cellStyle name="Titel" xfId="5" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="5" builtinId="15" customBuiltin="1"/>
     <cellStyle name="zHiddenText" xfId="3" xr:uid="{26E66EE6-E33F-4D77-BAE4-0FB4F5BBF673}"/>
   </cellStyles>
   <dxfs count="18">
@@ -1722,26 +1719,26 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BL36"/>
+  <dimension ref="A1:BL34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.75" style="13" customWidth="1"/>
-    <col min="2" max="2" width="40.125" customWidth="1"/>
-    <col min="3" max="3" width="16.75" customWidth="1"/>
-    <col min="4" max="4" width="10.75" customWidth="1"/>
-    <col min="5" max="5" width="10.75" style="2" customWidth="1"/>
-    <col min="6" max="6" width="10.75" customWidth="1"/>
-    <col min="7" max="7" width="2.75" customWidth="1"/>
+    <col min="1" max="1" width="2.69921875" style="13" customWidth="1"/>
+    <col min="2" max="2" width="40.09765625" customWidth="1"/>
+    <col min="3" max="3" width="16.69921875" customWidth="1"/>
+    <col min="4" max="4" width="10.69921875" customWidth="1"/>
+    <col min="5" max="5" width="10.69921875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.69921875" customWidth="1"/>
+    <col min="7" max="7" width="2.69921875" customWidth="1"/>
     <col min="8" max="8" width="6" hidden="1" customWidth="1"/>
-    <col min="9" max="65" width="2.75" customWidth="1"/>
+    <col min="9" max="65" width="2.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" ht="90" customHeight="1" x14ac:dyDescent="1.1000000000000001">
+    <row r="1" spans="1:64" ht="90" customHeight="1" x14ac:dyDescent="1.45">
       <c r="A1" s="14"/>
       <c r="B1" s="96" t="s">
         <v>25</v>
@@ -1751,30 +1748,30 @@
       <c r="E1" s="20"/>
       <c r="F1" s="21"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="112" t="s">
+      <c r="I1" s="113" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="113"/>
-      <c r="K1" s="113"/>
-      <c r="L1" s="113"/>
-      <c r="M1" s="113"/>
-      <c r="N1" s="113"/>
-      <c r="O1" s="113"/>
+      <c r="J1" s="114"/>
+      <c r="K1" s="114"/>
+      <c r="L1" s="114"/>
+      <c r="M1" s="114"/>
+      <c r="N1" s="114"/>
+      <c r="O1" s="114"/>
       <c r="P1" s="24"/>
-      <c r="Q1" s="111">
+      <c r="Q1" s="112">
         <v>45537</v>
       </c>
-      <c r="R1" s="110"/>
-      <c r="S1" s="110"/>
-      <c r="T1" s="110"/>
-      <c r="U1" s="110"/>
-      <c r="V1" s="110"/>
-      <c r="W1" s="110"/>
-      <c r="X1" s="110"/>
-      <c r="Y1" s="110"/>
-      <c r="Z1" s="110"/>
-    </row>
-    <row r="2" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="R1" s="111"/>
+      <c r="S1" s="111"/>
+      <c r="T1" s="111"/>
+      <c r="U1" s="111"/>
+      <c r="V1" s="111"/>
+      <c r="W1" s="111"/>
+      <c r="X1" s="111"/>
+      <c r="Y1" s="111"/>
+      <c r="Z1" s="111"/>
+    </row>
+    <row r="2" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B2" s="94" t="s">
         <v>26</v>
       </c>
@@ -1784,28 +1781,28 @@
       <c r="D2" s="22"/>
       <c r="E2" s="23"/>
       <c r="F2" s="22"/>
-      <c r="I2" s="112" t="s">
+      <c r="I2" s="113" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="113"/>
-      <c r="K2" s="113"/>
-      <c r="L2" s="113"/>
-      <c r="M2" s="113"/>
-      <c r="N2" s="113"/>
-      <c r="O2" s="113"/>
+      <c r="J2" s="114"/>
+      <c r="K2" s="114"/>
+      <c r="L2" s="114"/>
+      <c r="M2" s="114"/>
+      <c r="N2" s="114"/>
+      <c r="O2" s="114"/>
       <c r="P2" s="24"/>
-      <c r="Q2" s="109">
-        <v>2</v>
-      </c>
-      <c r="R2" s="110"/>
-      <c r="S2" s="110"/>
-      <c r="T2" s="110"/>
-      <c r="U2" s="110"/>
-      <c r="V2" s="110"/>
-      <c r="W2" s="110"/>
-      <c r="X2" s="110"/>
-      <c r="Y2" s="110"/>
-      <c r="Z2" s="110"/>
+      <c r="Q2" s="110">
+        <v>1</v>
+      </c>
+      <c r="R2" s="111"/>
+      <c r="S2" s="111"/>
+      <c r="T2" s="111"/>
+      <c r="U2" s="111"/>
+      <c r="V2" s="111"/>
+      <c r="W2" s="111"/>
+      <c r="X2" s="111"/>
+      <c r="Y2" s="111"/>
+      <c r="Z2" s="111"/>
     </row>
     <row r="3" spans="1:64" s="26" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
@@ -1815,568 +1812,568 @@
       <c r="D3" s="27"/>
       <c r="E3" s="28"/>
     </row>
-    <row r="4" spans="1:64" s="26" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:64" s="26" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14"/>
       <c r="B4" s="29" t="s">
         <v>13</v>
       </c>
       <c r="E4" s="30"/>
-      <c r="I4" s="106">
+      <c r="I4" s="117">
         <f>I5</f>
+        <v>45537</v>
+      </c>
+      <c r="J4" s="115"/>
+      <c r="K4" s="115"/>
+      <c r="L4" s="115"/>
+      <c r="M4" s="115"/>
+      <c r="N4" s="115"/>
+      <c r="O4" s="115"/>
+      <c r="P4" s="115">
+        <f>P5</f>
         <v>45544</v>
       </c>
-      <c r="J4" s="104"/>
-      <c r="K4" s="104"/>
-      <c r="L4" s="104"/>
-      <c r="M4" s="104"/>
-      <c r="N4" s="104"/>
-      <c r="O4" s="104"/>
-      <c r="P4" s="104">
-        <f>P5</f>
+      <c r="Q4" s="115"/>
+      <c r="R4" s="115"/>
+      <c r="S4" s="115"/>
+      <c r="T4" s="115"/>
+      <c r="U4" s="115"/>
+      <c r="V4" s="115"/>
+      <c r="W4" s="115">
+        <f>W5</f>
         <v>45551</v>
       </c>
-      <c r="Q4" s="104"/>
-      <c r="R4" s="104"/>
-      <c r="S4" s="104"/>
-      <c r="T4" s="104"/>
-      <c r="U4" s="104"/>
-      <c r="V4" s="104"/>
-      <c r="W4" s="104">
-        <f>W5</f>
+      <c r="X4" s="115"/>
+      <c r="Y4" s="115"/>
+      <c r="Z4" s="115"/>
+      <c r="AA4" s="115"/>
+      <c r="AB4" s="115"/>
+      <c r="AC4" s="115"/>
+      <c r="AD4" s="115">
+        <f>AD5</f>
         <v>45558</v>
       </c>
-      <c r="X4" s="104"/>
-      <c r="Y4" s="104"/>
-      <c r="Z4" s="104"/>
-      <c r="AA4" s="104"/>
-      <c r="AB4" s="104"/>
-      <c r="AC4" s="104"/>
-      <c r="AD4" s="104">
-        <f>AD5</f>
+      <c r="AE4" s="115"/>
+      <c r="AF4" s="115"/>
+      <c r="AG4" s="115"/>
+      <c r="AH4" s="115"/>
+      <c r="AI4" s="115"/>
+      <c r="AJ4" s="115"/>
+      <c r="AK4" s="115">
+        <f>AK5</f>
         <v>45565</v>
       </c>
-      <c r="AE4" s="104"/>
-      <c r="AF4" s="104"/>
-      <c r="AG4" s="104"/>
-      <c r="AH4" s="104"/>
-      <c r="AI4" s="104"/>
-      <c r="AJ4" s="104"/>
-      <c r="AK4" s="104">
-        <f>AK5</f>
+      <c r="AL4" s="115"/>
+      <c r="AM4" s="115"/>
+      <c r="AN4" s="115"/>
+      <c r="AO4" s="115"/>
+      <c r="AP4" s="115"/>
+      <c r="AQ4" s="115"/>
+      <c r="AR4" s="115">
+        <f>AR5</f>
         <v>45572</v>
       </c>
-      <c r="AL4" s="104"/>
-      <c r="AM4" s="104"/>
-      <c r="AN4" s="104"/>
-      <c r="AO4" s="104"/>
-      <c r="AP4" s="104"/>
-      <c r="AQ4" s="104"/>
-      <c r="AR4" s="104">
-        <f>AR5</f>
+      <c r="AS4" s="115"/>
+      <c r="AT4" s="115"/>
+      <c r="AU4" s="115"/>
+      <c r="AV4" s="115"/>
+      <c r="AW4" s="115"/>
+      <c r="AX4" s="115"/>
+      <c r="AY4" s="115">
+        <f>AY5</f>
         <v>45579</v>
       </c>
-      <c r="AS4" s="104"/>
-      <c r="AT4" s="104"/>
-      <c r="AU4" s="104"/>
-      <c r="AV4" s="104"/>
-      <c r="AW4" s="104"/>
-      <c r="AX4" s="104"/>
-      <c r="AY4" s="104">
-        <f>AY5</f>
+      <c r="AZ4" s="115"/>
+      <c r="BA4" s="115"/>
+      <c r="BB4" s="115"/>
+      <c r="BC4" s="115"/>
+      <c r="BD4" s="115"/>
+      <c r="BE4" s="115"/>
+      <c r="BF4" s="115">
+        <f>BF5</f>
         <v>45586</v>
       </c>
-      <c r="AZ4" s="104"/>
-      <c r="BA4" s="104"/>
-      <c r="BB4" s="104"/>
-      <c r="BC4" s="104"/>
-      <c r="BD4" s="104"/>
-      <c r="BE4" s="104"/>
-      <c r="BF4" s="104">
-        <f>BF5</f>
-        <v>45593</v>
-      </c>
-      <c r="BG4" s="104"/>
-      <c r="BH4" s="104"/>
-      <c r="BI4" s="104"/>
-      <c r="BJ4" s="104"/>
-      <c r="BK4" s="104"/>
-      <c r="BL4" s="105"/>
-    </row>
-    <row r="5" spans="1:64" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="114"/>
-      <c r="B5" s="115" t="s">
+      <c r="BG4" s="115"/>
+      <c r="BH4" s="115"/>
+      <c r="BI4" s="115"/>
+      <c r="BJ4" s="115"/>
+      <c r="BK4" s="115"/>
+      <c r="BL4" s="116"/>
+    </row>
+    <row r="5" spans="1:64" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="104"/>
+      <c r="B5" s="105" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="117" t="s">
+      <c r="C5" s="107" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="107" t="s">
+      <c r="D5" s="109" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="107" t="s">
+      <c r="E5" s="109" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="107" t="s">
+      <c r="F5" s="109" t="s">
         <v>4</v>
       </c>
       <c r="I5" s="31">
         <f>Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
-        <v>45544</v>
+        <v>45537</v>
       </c>
       <c r="J5" s="31">
         <f>I5+1</f>
-        <v>45545</v>
+        <v>45538</v>
       </c>
       <c r="K5" s="31">
         <f t="shared" ref="K5:AX5" si="0">J5+1</f>
-        <v>45546</v>
+        <v>45539</v>
       </c>
       <c r="L5" s="31">
         <f t="shared" si="0"/>
-        <v>45547</v>
+        <v>45540</v>
       </c>
       <c r="M5" s="31">
         <f t="shared" si="0"/>
-        <v>45548</v>
+        <v>45541</v>
       </c>
       <c r="N5" s="31">
         <f t="shared" si="0"/>
-        <v>45549</v>
+        <v>45542</v>
       </c>
       <c r="O5" s="32">
         <f t="shared" si="0"/>
-        <v>45550</v>
+        <v>45543</v>
       </c>
       <c r="P5" s="33">
         <f>O5+1</f>
-        <v>45551</v>
+        <v>45544</v>
       </c>
       <c r="Q5" s="31">
         <f>P5+1</f>
-        <v>45552</v>
+        <v>45545</v>
       </c>
       <c r="R5" s="31">
         <f t="shared" si="0"/>
-        <v>45553</v>
+        <v>45546</v>
       </c>
       <c r="S5" s="31">
         <f t="shared" si="0"/>
-        <v>45554</v>
+        <v>45547</v>
       </c>
       <c r="T5" s="31">
         <f t="shared" si="0"/>
-        <v>45555</v>
+        <v>45548</v>
       </c>
       <c r="U5" s="31">
         <f t="shared" si="0"/>
-        <v>45556</v>
+        <v>45549</v>
       </c>
       <c r="V5" s="32">
         <f t="shared" si="0"/>
-        <v>45557</v>
+        <v>45550</v>
       </c>
       <c r="W5" s="33">
         <f>V5+1</f>
-        <v>45558</v>
+        <v>45551</v>
       </c>
       <c r="X5" s="31">
         <f>W5+1</f>
-        <v>45559</v>
+        <v>45552</v>
       </c>
       <c r="Y5" s="31">
         <f t="shared" si="0"/>
-        <v>45560</v>
+        <v>45553</v>
       </c>
       <c r="Z5" s="31">
         <f t="shared" si="0"/>
-        <v>45561</v>
+        <v>45554</v>
       </c>
       <c r="AA5" s="31">
         <f t="shared" si="0"/>
-        <v>45562</v>
+        <v>45555</v>
       </c>
       <c r="AB5" s="31">
         <f t="shared" si="0"/>
-        <v>45563</v>
+        <v>45556</v>
       </c>
       <c r="AC5" s="32">
         <f t="shared" si="0"/>
-        <v>45564</v>
+        <v>45557</v>
       </c>
       <c r="AD5" s="33">
         <f>AC5+1</f>
-        <v>45565</v>
+        <v>45558</v>
       </c>
       <c r="AE5" s="31">
         <f>AD5+1</f>
-        <v>45566</v>
+        <v>45559</v>
       </c>
       <c r="AF5" s="31">
         <f t="shared" si="0"/>
-        <v>45567</v>
+        <v>45560</v>
       </c>
       <c r="AG5" s="31">
         <f t="shared" si="0"/>
-        <v>45568</v>
+        <v>45561</v>
       </c>
       <c r="AH5" s="31">
         <f t="shared" si="0"/>
-        <v>45569</v>
+        <v>45562</v>
       </c>
       <c r="AI5" s="31">
         <f t="shared" si="0"/>
-        <v>45570</v>
+        <v>45563</v>
       </c>
       <c r="AJ5" s="32">
         <f t="shared" si="0"/>
-        <v>45571</v>
+        <v>45564</v>
       </c>
       <c r="AK5" s="33">
         <f>AJ5+1</f>
-        <v>45572</v>
+        <v>45565</v>
       </c>
       <c r="AL5" s="31">
         <f>AK5+1</f>
-        <v>45573</v>
+        <v>45566</v>
       </c>
       <c r="AM5" s="31">
         <f t="shared" si="0"/>
-        <v>45574</v>
+        <v>45567</v>
       </c>
       <c r="AN5" s="31">
         <f t="shared" si="0"/>
-        <v>45575</v>
+        <v>45568</v>
       </c>
       <c r="AO5" s="31">
         <f t="shared" si="0"/>
-        <v>45576</v>
+        <v>45569</v>
       </c>
       <c r="AP5" s="31">
         <f t="shared" si="0"/>
-        <v>45577</v>
+        <v>45570</v>
       </c>
       <c r="AQ5" s="32">
         <f t="shared" si="0"/>
-        <v>45578</v>
+        <v>45571</v>
       </c>
       <c r="AR5" s="33">
         <f>AQ5+1</f>
-        <v>45579</v>
+        <v>45572</v>
       </c>
       <c r="AS5" s="31">
         <f>AR5+1</f>
-        <v>45580</v>
+        <v>45573</v>
       </c>
       <c r="AT5" s="31">
         <f t="shared" si="0"/>
-        <v>45581</v>
+        <v>45574</v>
       </c>
       <c r="AU5" s="31">
         <f t="shared" si="0"/>
-        <v>45582</v>
+        <v>45575</v>
       </c>
       <c r="AV5" s="31">
         <f t="shared" si="0"/>
-        <v>45583</v>
+        <v>45576</v>
       </c>
       <c r="AW5" s="31">
         <f t="shared" si="0"/>
-        <v>45584</v>
+        <v>45577</v>
       </c>
       <c r="AX5" s="32">
         <f t="shared" si="0"/>
-        <v>45585</v>
+        <v>45578</v>
       </c>
       <c r="AY5" s="33">
         <f>AX5+1</f>
-        <v>45586</v>
+        <v>45579</v>
       </c>
       <c r="AZ5" s="31">
         <f>AY5+1</f>
-        <v>45587</v>
+        <v>45580</v>
       </c>
       <c r="BA5" s="31">
         <f t="shared" ref="BA5:BE5" si="1">AZ5+1</f>
-        <v>45588</v>
+        <v>45581</v>
       </c>
       <c r="BB5" s="31">
         <f t="shared" si="1"/>
-        <v>45589</v>
+        <v>45582</v>
       </c>
       <c r="BC5" s="31">
         <f t="shared" si="1"/>
-        <v>45590</v>
+        <v>45583</v>
       </c>
       <c r="BD5" s="31">
         <f t="shared" si="1"/>
-        <v>45591</v>
+        <v>45584</v>
       </c>
       <c r="BE5" s="32">
         <f t="shared" si="1"/>
-        <v>45592</v>
+        <v>45585</v>
       </c>
       <c r="BF5" s="33">
         <f>BE5+1</f>
-        <v>45593</v>
+        <v>45586</v>
       </c>
       <c r="BG5" s="31">
         <f>BF5+1</f>
-        <v>45594</v>
+        <v>45587</v>
       </c>
       <c r="BH5" s="31">
         <f t="shared" ref="BH5:BL5" si="2">BG5+1</f>
-        <v>45595</v>
+        <v>45588</v>
       </c>
       <c r="BI5" s="31">
         <f t="shared" si="2"/>
-        <v>45596</v>
+        <v>45589</v>
       </c>
       <c r="BJ5" s="31">
         <f t="shared" si="2"/>
-        <v>45597</v>
+        <v>45590</v>
       </c>
       <c r="BK5" s="31">
         <f t="shared" si="2"/>
-        <v>45598</v>
+        <v>45591</v>
       </c>
       <c r="BL5" s="31">
         <f t="shared" si="2"/>
-        <v>45599</v>
-      </c>
-    </row>
-    <row r="6" spans="1:64" s="26" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="114"/>
-      <c r="B6" s="116"/>
+        <v>45592</v>
+      </c>
+    </row>
+    <row r="6" spans="1:64" s="26" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="104"/>
+      <c r="B6" s="106"/>
       <c r="C6" s="108"/>
       <c r="D6" s="108"/>
       <c r="E6" s="108"/>
       <c r="F6" s="108"/>
       <c r="I6" s="34" t="str">
         <f t="shared" ref="I6:AN6" si="3">LEFT(TEXT(I5,"ddd"),1)</f>
-        <v>M</v>
+        <v>m</v>
       </c>
       <c r="J6" s="35" t="str">
         <f t="shared" si="3"/>
-        <v>T</v>
+        <v>t</v>
       </c>
       <c r="K6" s="35" t="str">
         <f t="shared" si="3"/>
-        <v>W</v>
+        <v>o</v>
       </c>
       <c r="L6" s="35" t="str">
         <f t="shared" si="3"/>
-        <v>T</v>
+        <v>t</v>
       </c>
       <c r="M6" s="35" t="str">
         <f t="shared" si="3"/>
-        <v>F</v>
+        <v>f</v>
       </c>
       <c r="N6" s="35" t="str">
         <f t="shared" si="3"/>
-        <v>S</v>
+        <v>l</v>
       </c>
       <c r="O6" s="35" t="str">
         <f t="shared" si="3"/>
-        <v>S</v>
+        <v>s</v>
       </c>
       <c r="P6" s="35" t="str">
         <f t="shared" si="3"/>
-        <v>M</v>
+        <v>m</v>
       </c>
       <c r="Q6" s="35" t="str">
         <f t="shared" si="3"/>
-        <v>T</v>
+        <v>t</v>
       </c>
       <c r="R6" s="35" t="str">
         <f t="shared" si="3"/>
-        <v>W</v>
+        <v>o</v>
       </c>
       <c r="S6" s="35" t="str">
         <f t="shared" si="3"/>
-        <v>T</v>
+        <v>t</v>
       </c>
       <c r="T6" s="35" t="str">
         <f t="shared" si="3"/>
-        <v>F</v>
+        <v>f</v>
       </c>
       <c r="U6" s="35" t="str">
         <f t="shared" si="3"/>
-        <v>S</v>
+        <v>l</v>
       </c>
       <c r="V6" s="35" t="str">
         <f t="shared" si="3"/>
-        <v>S</v>
+        <v>s</v>
       </c>
       <c r="W6" s="35" t="str">
         <f t="shared" si="3"/>
-        <v>M</v>
+        <v>m</v>
       </c>
       <c r="X6" s="35" t="str">
         <f t="shared" si="3"/>
-        <v>T</v>
+        <v>t</v>
       </c>
       <c r="Y6" s="35" t="str">
         <f t="shared" si="3"/>
-        <v>W</v>
+        <v>o</v>
       </c>
       <c r="Z6" s="35" t="str">
         <f t="shared" si="3"/>
-        <v>T</v>
+        <v>t</v>
       </c>
       <c r="AA6" s="35" t="str">
         <f t="shared" si="3"/>
-        <v>F</v>
+        <v>f</v>
       </c>
       <c r="AB6" s="35" t="str">
         <f t="shared" si="3"/>
-        <v>S</v>
+        <v>l</v>
       </c>
       <c r="AC6" s="35" t="str">
         <f t="shared" si="3"/>
-        <v>S</v>
+        <v>s</v>
       </c>
       <c r="AD6" s="35" t="str">
         <f t="shared" si="3"/>
-        <v>M</v>
+        <v>m</v>
       </c>
       <c r="AE6" s="35" t="str">
         <f t="shared" si="3"/>
-        <v>T</v>
+        <v>t</v>
       </c>
       <c r="AF6" s="35" t="str">
         <f t="shared" si="3"/>
-        <v>W</v>
+        <v>o</v>
       </c>
       <c r="AG6" s="35" t="str">
         <f t="shared" si="3"/>
-        <v>T</v>
+        <v>t</v>
       </c>
       <c r="AH6" s="35" t="str">
         <f t="shared" si="3"/>
-        <v>F</v>
+        <v>f</v>
       </c>
       <c r="AI6" s="35" t="str">
         <f t="shared" si="3"/>
-        <v>S</v>
+        <v>l</v>
       </c>
       <c r="AJ6" s="35" t="str">
         <f t="shared" si="3"/>
-        <v>S</v>
+        <v>s</v>
       </c>
       <c r="AK6" s="35" t="str">
         <f t="shared" si="3"/>
-        <v>M</v>
+        <v>m</v>
       </c>
       <c r="AL6" s="35" t="str">
         <f t="shared" si="3"/>
-        <v>T</v>
+        <v>t</v>
       </c>
       <c r="AM6" s="35" t="str">
         <f t="shared" si="3"/>
-        <v>W</v>
+        <v>o</v>
       </c>
       <c r="AN6" s="35" t="str">
         <f t="shared" si="3"/>
-        <v>T</v>
+        <v>t</v>
       </c>
       <c r="AO6" s="35" t="str">
         <f t="shared" ref="AO6:BL6" si="4">LEFT(TEXT(AO5,"ddd"),1)</f>
-        <v>F</v>
+        <v>f</v>
       </c>
       <c r="AP6" s="35" t="str">
         <f t="shared" si="4"/>
-        <v>S</v>
+        <v>l</v>
       </c>
       <c r="AQ6" s="35" t="str">
         <f t="shared" si="4"/>
-        <v>S</v>
+        <v>s</v>
       </c>
       <c r="AR6" s="35" t="str">
         <f t="shared" si="4"/>
-        <v>M</v>
+        <v>m</v>
       </c>
       <c r="AS6" s="35" t="str">
         <f t="shared" si="4"/>
-        <v>T</v>
+        <v>t</v>
       </c>
       <c r="AT6" s="35" t="str">
         <f t="shared" si="4"/>
-        <v>W</v>
+        <v>o</v>
       </c>
       <c r="AU6" s="35" t="str">
         <f t="shared" si="4"/>
-        <v>T</v>
+        <v>t</v>
       </c>
       <c r="AV6" s="35" t="str">
         <f t="shared" si="4"/>
-        <v>F</v>
+        <v>f</v>
       </c>
       <c r="AW6" s="35" t="str">
         <f t="shared" si="4"/>
-        <v>S</v>
+        <v>l</v>
       </c>
       <c r="AX6" s="35" t="str">
         <f t="shared" si="4"/>
-        <v>S</v>
+        <v>s</v>
       </c>
       <c r="AY6" s="35" t="str">
         <f t="shared" si="4"/>
-        <v>M</v>
+        <v>m</v>
       </c>
       <c r="AZ6" s="35" t="str">
         <f t="shared" si="4"/>
-        <v>T</v>
+        <v>t</v>
       </c>
       <c r="BA6" s="35" t="str">
         <f t="shared" si="4"/>
-        <v>W</v>
+        <v>o</v>
       </c>
       <c r="BB6" s="35" t="str">
         <f t="shared" si="4"/>
-        <v>T</v>
+        <v>t</v>
       </c>
       <c r="BC6" s="35" t="str">
         <f t="shared" si="4"/>
-        <v>F</v>
+        <v>f</v>
       </c>
       <c r="BD6" s="35" t="str">
         <f t="shared" si="4"/>
-        <v>S</v>
+        <v>l</v>
       </c>
       <c r="BE6" s="35" t="str">
         <f t="shared" si="4"/>
-        <v>S</v>
+        <v>s</v>
       </c>
       <c r="BF6" s="35" t="str">
         <f t="shared" si="4"/>
-        <v>M</v>
+        <v>m</v>
       </c>
       <c r="BG6" s="35" t="str">
         <f t="shared" si="4"/>
-        <v>T</v>
+        <v>t</v>
       </c>
       <c r="BH6" s="35" t="str">
         <f t="shared" si="4"/>
-        <v>W</v>
+        <v>o</v>
       </c>
       <c r="BI6" s="35" t="str">
         <f t="shared" si="4"/>
-        <v>T</v>
+        <v>t</v>
       </c>
       <c r="BJ6" s="35" t="str">
         <f t="shared" si="4"/>
-        <v>F</v>
+        <v>f</v>
       </c>
       <c r="BK6" s="35" t="str">
         <f t="shared" si="4"/>
-        <v>S</v>
+        <v>l</v>
       </c>
       <c r="BL6" s="36" t="str">
         <f t="shared" si="4"/>
-        <v>S</v>
-      </c>
-    </row>
-    <row r="7" spans="1:64" s="26" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>s</v>
+      </c>
+    </row>
+    <row r="7" spans="1:64" s="26" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>20</v>
       </c>
@@ -2446,7 +2443,7 @@
       <c r="BK7" s="39"/>
       <c r="BL7" s="39"/>
     </row>
-    <row r="8" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="14"/>
       <c r="B8" s="40" t="s">
         <v>28</v>
@@ -2457,7 +2454,7 @@
       <c r="F8" s="44"/>
       <c r="G8" s="17"/>
       <c r="H8" s="5" t="str">
-        <f t="shared" ref="H8:H33" si="5">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="H8:H31" si="5">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
       <c r="I8" s="45"/>
@@ -2517,7 +2514,7 @@
       <c r="BK8" s="45"/>
       <c r="BL8" s="45"/>
     </row>
-    <row r="9" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="14"/>
       <c r="B9" s="47" t="s">
         <v>21</v>
@@ -2526,7 +2523,7 @@
         <v>27</v>
       </c>
       <c r="D9" s="49">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E9" s="50">
         <f>Project_Start</f>
@@ -2597,16 +2594,16 @@
       <c r="BK9" s="51"/>
       <c r="BL9" s="51"/>
     </row>
-    <row r="10" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="14"/>
       <c r="B10" s="52" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C10" s="48" t="s">
         <v>27</v>
       </c>
       <c r="D10" s="49">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="E10" s="53">
         <f>E9</f>
@@ -2678,7 +2675,7 @@
       <c r="BK10" s="51"/>
       <c r="BL10" s="51"/>
     </row>
-    <row r="11" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="13"/>
       <c r="B11" s="52" t="s">
         <v>30</v>
@@ -2687,7 +2684,7 @@
         <v>27</v>
       </c>
       <c r="D11" s="49">
-        <v>0.15</v>
+        <v>0.9</v>
       </c>
       <c r="E11" s="53">
         <v>45550</v>
@@ -2758,7 +2755,7 @@
       <c r="BK11" s="51"/>
       <c r="BL11" s="51"/>
     </row>
-    <row r="12" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="13"/>
       <c r="B12" s="52" t="s">
         <v>29</v>
@@ -2767,7 +2764,7 @@
         <v>27</v>
       </c>
       <c r="D12" s="49">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="E12" s="53">
         <f>F10-7</f>
@@ -2839,7 +2836,7 @@
       <c r="BK12" s="51"/>
       <c r="BL12" s="51"/>
     </row>
-    <row r="13" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="13"/>
       <c r="B13" s="52" t="s">
         <v>34</v>
@@ -2848,7 +2845,7 @@
         <v>27</v>
       </c>
       <c r="D13" s="49">
-        <v>0.15</v>
+        <v>0.85</v>
       </c>
       <c r="E13" s="53">
         <f xml:space="preserve"> E11</f>
@@ -2920,7 +2917,7 @@
       <c r="BK13" s="51"/>
       <c r="BL13" s="51"/>
     </row>
-    <row r="14" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="14"/>
       <c r="B14" s="55" t="s">
         <v>31</v>
@@ -2935,16 +2932,16 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="60" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C15" s="61" t="s">
         <v>27</v>
       </c>
       <c r="D15" s="62">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="E15" s="63">
         <f>F12</f>
@@ -3016,16 +3013,16 @@
       <c r="BK15" s="51"/>
       <c r="BL15" s="51"/>
     </row>
-    <row r="16" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="13"/>
       <c r="B16" s="60" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C16" s="61" t="s">
         <v>27</v>
       </c>
       <c r="D16" s="62">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="E16" s="63">
         <f>E15</f>
@@ -3097,10 +3094,10 @@
       <c r="BK16" s="51"/>
       <c r="BL16" s="51"/>
     </row>
-    <row r="17" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="13"/>
       <c r="B17" s="60" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C17" s="61" t="s">
         <v>27</v>
@@ -3178,19 +3175,19 @@
       <c r="BK17" s="51"/>
       <c r="BL17" s="51"/>
     </row>
-    <row r="18" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="13"/>
       <c r="B18" s="60" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C18" s="61" t="s">
         <v>27</v>
       </c>
       <c r="D18" s="62">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="E18" s="63">
-        <f t="shared" ref="E18" si="7">E15</f>
+        <f t="shared" ref="E18" si="7">E17</f>
         <v>45571</v>
       </c>
       <c r="F18" s="63">
@@ -3218,7 +3215,7 @@
       <c r="V18" s="51"/>
       <c r="W18" s="51"/>
       <c r="X18" s="51"/>
-      <c r="Y18" s="54"/>
+      <c r="Y18" s="51"/>
       <c r="Z18" s="51"/>
       <c r="AA18" s="51"/>
       <c r="AB18" s="51"/>
@@ -3259,162 +3256,162 @@
       <c r="BK18" s="51"/>
       <c r="BL18" s="51"/>
     </row>
-    <row r="19" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="13"/>
-      <c r="B19" s="60" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" s="61" t="s">
-        <v>27</v>
-      </c>
-      <c r="D19" s="62">
-        <v>0</v>
-      </c>
-      <c r="E19" s="63">
-        <f t="shared" ref="E19" si="8">E17</f>
-        <v>45571</v>
-      </c>
-      <c r="F19" s="63">
-        <f>E19+14</f>
-        <v>45585</v>
-      </c>
+      <c r="B19" s="64" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="65"/>
+      <c r="D19" s="66"/>
+      <c r="E19" s="67"/>
+      <c r="F19" s="68"/>
       <c r="G19" s="17"/>
-      <c r="H19" s="5">
-        <f t="shared" si="5"/>
-        <v>15</v>
-      </c>
-      <c r="I19" s="51"/>
-      <c r="J19" s="51"/>
-      <c r="K19" s="51"/>
-      <c r="L19" s="51"/>
-      <c r="M19" s="51"/>
-      <c r="N19" s="51"/>
-      <c r="O19" s="51"/>
-      <c r="P19" s="51"/>
-      <c r="Q19" s="51"/>
-      <c r="R19" s="51"/>
-      <c r="S19" s="51"/>
-      <c r="T19" s="51"/>
-      <c r="U19" s="51"/>
-      <c r="V19" s="51"/>
-      <c r="W19" s="51"/>
-      <c r="X19" s="51"/>
-      <c r="Y19" s="51"/>
-      <c r="Z19" s="51"/>
-      <c r="AA19" s="51"/>
-      <c r="AB19" s="51"/>
-      <c r="AC19" s="51"/>
-      <c r="AD19" s="51"/>
-      <c r="AE19" s="51"/>
-      <c r="AF19" s="51"/>
-      <c r="AG19" s="51"/>
-      <c r="AH19" s="51"/>
-      <c r="AI19" s="51"/>
-      <c r="AJ19" s="51"/>
-      <c r="AK19" s="51"/>
-      <c r="AL19" s="51"/>
-      <c r="AM19" s="51"/>
-      <c r="AN19" s="51"/>
-      <c r="AO19" s="51"/>
-      <c r="AP19" s="51"/>
-      <c r="AQ19" s="51"/>
-      <c r="AR19" s="51"/>
-      <c r="AS19" s="51"/>
-      <c r="AT19" s="51"/>
-      <c r="AU19" s="51"/>
-      <c r="AV19" s="51"/>
-      <c r="AW19" s="51"/>
-      <c r="AX19" s="51"/>
-      <c r="AY19" s="51"/>
-      <c r="AZ19" s="51"/>
-      <c r="BA19" s="51"/>
-      <c r="BB19" s="51"/>
-      <c r="BC19" s="51"/>
-      <c r="BD19" s="51"/>
-      <c r="BE19" s="51"/>
-      <c r="BF19" s="51"/>
-      <c r="BG19" s="51"/>
-      <c r="BH19" s="51"/>
-      <c r="BI19" s="51"/>
-      <c r="BJ19" s="51"/>
-      <c r="BK19" s="51"/>
-      <c r="BL19" s="51"/>
-    </row>
-    <row r="20" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
-      <c r="B20" s="64" t="s">
-        <v>32</v>
-      </c>
-      <c r="C20" s="65"/>
-      <c r="D20" s="66"/>
-      <c r="E20" s="67"/>
-      <c r="F20" s="68"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="5" t="str">
+      <c r="H19" s="5" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="I20" s="69"/>
-      <c r="J20" s="69"/>
-      <c r="K20" s="69"/>
-      <c r="L20" s="69"/>
-      <c r="M20" s="69"/>
-      <c r="N20" s="69"/>
-      <c r="O20" s="69"/>
-      <c r="P20" s="69"/>
-      <c r="Q20" s="69"/>
-      <c r="R20" s="69"/>
-      <c r="S20" s="69"/>
-      <c r="T20" s="69"/>
-      <c r="U20" s="69"/>
-      <c r="V20" s="69"/>
-      <c r="W20" s="69"/>
-      <c r="X20" s="69"/>
-      <c r="Y20" s="69"/>
-      <c r="Z20" s="69"/>
-      <c r="AA20" s="69"/>
-      <c r="AB20" s="69"/>
-      <c r="AC20" s="69"/>
-      <c r="AD20" s="69"/>
-      <c r="AE20" s="69"/>
-      <c r="AF20" s="69"/>
-      <c r="AG20" s="69"/>
-      <c r="AH20" s="69"/>
-      <c r="AI20" s="69"/>
-      <c r="AJ20" s="69"/>
-      <c r="AK20" s="69"/>
-      <c r="AL20" s="69"/>
-      <c r="AM20" s="69"/>
-      <c r="AN20" s="69"/>
-      <c r="AO20" s="69"/>
-      <c r="AP20" s="69"/>
-      <c r="AQ20" s="69"/>
-      <c r="AR20" s="69"/>
-      <c r="AS20" s="69"/>
-      <c r="AT20" s="69"/>
-      <c r="AU20" s="69"/>
-      <c r="AV20" s="69"/>
-      <c r="AW20" s="69"/>
-      <c r="AX20" s="69"/>
-      <c r="AY20" s="69"/>
-      <c r="AZ20" s="69"/>
-      <c r="BA20" s="69"/>
-      <c r="BB20" s="69"/>
-      <c r="BC20" s="69"/>
-      <c r="BD20" s="69"/>
-      <c r="BE20" s="69"/>
-      <c r="BF20" s="69"/>
-      <c r="BG20" s="69"/>
-      <c r="BH20" s="69"/>
-      <c r="BI20" s="69"/>
-      <c r="BJ20" s="69"/>
-      <c r="BK20" s="69"/>
-      <c r="BL20" s="69"/>
-    </row>
-    <row r="21" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I19" s="69"/>
+      <c r="J19" s="69"/>
+      <c r="K19" s="69"/>
+      <c r="L19" s="69"/>
+      <c r="M19" s="69"/>
+      <c r="N19" s="69"/>
+      <c r="O19" s="69"/>
+      <c r="P19" s="69"/>
+      <c r="Q19" s="69"/>
+      <c r="R19" s="69"/>
+      <c r="S19" s="69"/>
+      <c r="T19" s="69"/>
+      <c r="U19" s="69"/>
+      <c r="V19" s="69"/>
+      <c r="W19" s="69"/>
+      <c r="X19" s="69"/>
+      <c r="Y19" s="69"/>
+      <c r="Z19" s="69"/>
+      <c r="AA19" s="69"/>
+      <c r="AB19" s="69"/>
+      <c r="AC19" s="69"/>
+      <c r="AD19" s="69"/>
+      <c r="AE19" s="69"/>
+      <c r="AF19" s="69"/>
+      <c r="AG19" s="69"/>
+      <c r="AH19" s="69"/>
+      <c r="AI19" s="69"/>
+      <c r="AJ19" s="69"/>
+      <c r="AK19" s="69"/>
+      <c r="AL19" s="69"/>
+      <c r="AM19" s="69"/>
+      <c r="AN19" s="69"/>
+      <c r="AO19" s="69"/>
+      <c r="AP19" s="69"/>
+      <c r="AQ19" s="69"/>
+      <c r="AR19" s="69"/>
+      <c r="AS19" s="69"/>
+      <c r="AT19" s="69"/>
+      <c r="AU19" s="69"/>
+      <c r="AV19" s="69"/>
+      <c r="AW19" s="69"/>
+      <c r="AX19" s="69"/>
+      <c r="AY19" s="69"/>
+      <c r="AZ19" s="69"/>
+      <c r="BA19" s="69"/>
+      <c r="BB19" s="69"/>
+      <c r="BC19" s="69"/>
+      <c r="BD19" s="69"/>
+      <c r="BE19" s="69"/>
+      <c r="BF19" s="69"/>
+      <c r="BG19" s="69"/>
+      <c r="BH19" s="69"/>
+      <c r="BI19" s="69"/>
+      <c r="BJ19" s="69"/>
+      <c r="BK19" s="69"/>
+      <c r="BL19" s="69"/>
+    </row>
+    <row r="20" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="13"/>
+      <c r="B20" s="70" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="71" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="72">
+        <v>0.2</v>
+      </c>
+      <c r="E20" s="73">
+        <f xml:space="preserve"> F18</f>
+        <v>45585</v>
+      </c>
+      <c r="F20" s="73">
+        <f>E20+28</f>
+        <v>45613</v>
+      </c>
+      <c r="G20" s="17"/>
+      <c r="H20" s="5">
+        <f t="shared" si="5"/>
+        <v>29</v>
+      </c>
+      <c r="I20" s="51"/>
+      <c r="J20" s="51"/>
+      <c r="K20" s="51"/>
+      <c r="L20" s="51"/>
+      <c r="M20" s="51"/>
+      <c r="N20" s="51"/>
+      <c r="O20" s="51"/>
+      <c r="P20" s="51"/>
+      <c r="Q20" s="51"/>
+      <c r="R20" s="51"/>
+      <c r="S20" s="51"/>
+      <c r="T20" s="51"/>
+      <c r="U20" s="51"/>
+      <c r="V20" s="51"/>
+      <c r="W20" s="51"/>
+      <c r="X20" s="51"/>
+      <c r="Y20" s="51"/>
+      <c r="Z20" s="51"/>
+      <c r="AA20" s="51"/>
+      <c r="AB20" s="51"/>
+      <c r="AC20" s="51"/>
+      <c r="AD20" s="51"/>
+      <c r="AE20" s="51"/>
+      <c r="AF20" s="51"/>
+      <c r="AG20" s="51"/>
+      <c r="AH20" s="51"/>
+      <c r="AI20" s="51"/>
+      <c r="AJ20" s="51"/>
+      <c r="AK20" s="51"/>
+      <c r="AL20" s="51"/>
+      <c r="AM20" s="51"/>
+      <c r="AN20" s="51"/>
+      <c r="AO20" s="51"/>
+      <c r="AP20" s="51"/>
+      <c r="AQ20" s="51"/>
+      <c r="AR20" s="51"/>
+      <c r="AS20" s="51"/>
+      <c r="AT20" s="51"/>
+      <c r="AU20" s="51"/>
+      <c r="AV20" s="51"/>
+      <c r="AW20" s="51"/>
+      <c r="AX20" s="51"/>
+      <c r="AY20" s="51"/>
+      <c r="AZ20" s="51"/>
+      <c r="BA20" s="51"/>
+      <c r="BB20" s="51"/>
+      <c r="BC20" s="51"/>
+      <c r="BD20" s="51"/>
+      <c r="BE20" s="51"/>
+      <c r="BF20" s="51"/>
+      <c r="BG20" s="51"/>
+      <c r="BH20" s="51"/>
+      <c r="BI20" s="51"/>
+      <c r="BJ20" s="51"/>
+      <c r="BK20" s="51"/>
+      <c r="BL20" s="51"/>
+    </row>
+    <row r="21" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="13"/>
       <c r="B21" s="70" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C21" s="71" t="s">
         <v>27</v>
@@ -3423,7 +3420,7 @@
         <v>0</v>
       </c>
       <c r="E21" s="73">
-        <f xml:space="preserve"> F19</f>
+        <f xml:space="preserve"> F18</f>
         <v>45585</v>
       </c>
       <c r="F21" s="73">
@@ -3492,10 +3489,10 @@
       <c r="BK21" s="51"/>
       <c r="BL21" s="51"/>
     </row>
-    <row r="22" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="13"/>
       <c r="B22" s="70" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="C22" s="71" t="s">
         <v>27</v>
@@ -3504,17 +3501,17 @@
         <v>0</v>
       </c>
       <c r="E22" s="73">
-        <f xml:space="preserve"> F19</f>
-        <v>45585</v>
+        <f>F25</f>
+        <v>45627</v>
       </c>
       <c r="F22" s="73">
-        <f>E22+28</f>
-        <v>45613</v>
+        <f>E22+32</f>
+        <v>45659</v>
       </c>
       <c r="G22" s="17"/>
       <c r="H22" s="5">
         <f t="shared" si="5"/>
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="I22" s="51"/>
       <c r="J22" s="51"/>
@@ -3573,10 +3570,10 @@
       <c r="BK22" s="51"/>
       <c r="BL22" s="51"/>
     </row>
-    <row r="23" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="13"/>
       <c r="B23" s="70" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C23" s="71" t="s">
         <v>27</v>
@@ -3585,7 +3582,7 @@
         <v>0</v>
       </c>
       <c r="E23" s="73">
-        <f>F27</f>
+        <f>F25</f>
         <v>45627</v>
       </c>
       <c r="F23" s="73">
@@ -3654,108 +3651,100 @@
       <c r="BK23" s="51"/>
       <c r="BL23" s="51"/>
     </row>
-    <row r="24" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="13"/>
-      <c r="B24" s="70" t="s">
-        <v>44</v>
-      </c>
-      <c r="C24" s="71" t="s">
+      <c r="B24" s="74" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" s="75"/>
+      <c r="D24" s="76"/>
+      <c r="E24" s="77"/>
+      <c r="F24" s="78"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="5" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="I24" s="79"/>
+      <c r="J24" s="79"/>
+      <c r="K24" s="79"/>
+      <c r="L24" s="79"/>
+      <c r="M24" s="79"/>
+      <c r="N24" s="79"/>
+      <c r="O24" s="79"/>
+      <c r="P24" s="79"/>
+      <c r="Q24" s="79"/>
+      <c r="R24" s="79"/>
+      <c r="S24" s="79"/>
+      <c r="T24" s="79"/>
+      <c r="U24" s="79"/>
+      <c r="V24" s="79"/>
+      <c r="W24" s="79"/>
+      <c r="X24" s="79"/>
+      <c r="Y24" s="79"/>
+      <c r="Z24" s="79"/>
+      <c r="AA24" s="79"/>
+      <c r="AB24" s="79"/>
+      <c r="AC24" s="79"/>
+      <c r="AD24" s="79"/>
+      <c r="AE24" s="79"/>
+      <c r="AF24" s="79"/>
+      <c r="AG24" s="79"/>
+      <c r="AH24" s="79"/>
+      <c r="AI24" s="79"/>
+      <c r="AJ24" s="79"/>
+      <c r="AK24" s="79"/>
+      <c r="AL24" s="79"/>
+      <c r="AM24" s="79"/>
+      <c r="AN24" s="79"/>
+      <c r="AO24" s="79"/>
+      <c r="AP24" s="79"/>
+      <c r="AQ24" s="79"/>
+      <c r="AR24" s="79"/>
+      <c r="AS24" s="79"/>
+      <c r="AT24" s="79"/>
+      <c r="AU24" s="79"/>
+      <c r="AV24" s="79"/>
+      <c r="AW24" s="79"/>
+      <c r="AX24" s="79"/>
+      <c r="AY24" s="79"/>
+      <c r="AZ24" s="79"/>
+      <c r="BA24" s="79"/>
+      <c r="BB24" s="79"/>
+      <c r="BC24" s="79"/>
+      <c r="BD24" s="79"/>
+      <c r="BE24" s="79"/>
+      <c r="BF24" s="79"/>
+      <c r="BG24" s="79"/>
+      <c r="BH24" s="79"/>
+      <c r="BI24" s="79"/>
+      <c r="BJ24" s="79"/>
+      <c r="BK24" s="79"/>
+      <c r="BL24" s="79"/>
+    </row>
+    <row r="25" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="13"/>
+      <c r="B25" s="80" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" s="81" t="s">
         <v>27</v>
       </c>
-      <c r="D24" s="72">
+      <c r="D25" s="82">
         <v>0</v>
       </c>
-      <c r="E24" s="73">
-        <f>F27</f>
+      <c r="E25" s="83">
+        <f xml:space="preserve"> F21</f>
+        <v>45613</v>
+      </c>
+      <c r="F25" s="83">
+        <f>E25+14</f>
         <v>45627</v>
-      </c>
-      <c r="F24" s="73">
-        <f>E24+32</f>
-        <v>45659</v>
-      </c>
-      <c r="G24" s="17"/>
-      <c r="H24" s="5">
-        <f t="shared" si="5"/>
-        <v>33</v>
-      </c>
-      <c r="I24" s="51"/>
-      <c r="J24" s="51"/>
-      <c r="K24" s="51"/>
-      <c r="L24" s="51"/>
-      <c r="M24" s="51"/>
-      <c r="N24" s="51"/>
-      <c r="O24" s="51"/>
-      <c r="P24" s="51"/>
-      <c r="Q24" s="51"/>
-      <c r="R24" s="51"/>
-      <c r="S24" s="51"/>
-      <c r="T24" s="51"/>
-      <c r="U24" s="51"/>
-      <c r="V24" s="51"/>
-      <c r="W24" s="51"/>
-      <c r="X24" s="51"/>
-      <c r="Y24" s="51"/>
-      <c r="Z24" s="51"/>
-      <c r="AA24" s="51"/>
-      <c r="AB24" s="51"/>
-      <c r="AC24" s="51"/>
-      <c r="AD24" s="51"/>
-      <c r="AE24" s="51"/>
-      <c r="AF24" s="51"/>
-      <c r="AG24" s="51"/>
-      <c r="AH24" s="51"/>
-      <c r="AI24" s="51"/>
-      <c r="AJ24" s="51"/>
-      <c r="AK24" s="51"/>
-      <c r="AL24" s="51"/>
-      <c r="AM24" s="51"/>
-      <c r="AN24" s="51"/>
-      <c r="AO24" s="51"/>
-      <c r="AP24" s="51"/>
-      <c r="AQ24" s="51"/>
-      <c r="AR24" s="51"/>
-      <c r="AS24" s="51"/>
-      <c r="AT24" s="51"/>
-      <c r="AU24" s="51"/>
-      <c r="AV24" s="51"/>
-      <c r="AW24" s="51"/>
-      <c r="AX24" s="51"/>
-      <c r="AY24" s="51"/>
-      <c r="AZ24" s="51"/>
-      <c r="BA24" s="51"/>
-      <c r="BB24" s="51"/>
-      <c r="BC24" s="51"/>
-      <c r="BD24" s="51"/>
-      <c r="BE24" s="51"/>
-      <c r="BF24" s="51"/>
-      <c r="BG24" s="51"/>
-      <c r="BH24" s="51"/>
-      <c r="BI24" s="51"/>
-      <c r="BJ24" s="51"/>
-      <c r="BK24" s="51"/>
-      <c r="BL24" s="51"/>
-    </row>
-    <row r="25" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="13"/>
-      <c r="B25" s="70"/>
-      <c r="C25" s="71" t="s">
-        <v>27</v>
-      </c>
-      <c r="D25" s="72">
-        <v>0</v>
-      </c>
-      <c r="E25" s="73">
-        <f>F27</f>
-        <v>45627</v>
-      </c>
-      <c r="F25" s="73">
-        <f>E25+28</f>
-        <v>45655</v>
       </c>
       <c r="G25" s="17"/>
       <c r="H25" s="5">
         <f t="shared" si="5"/>
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="I25" s="51"/>
       <c r="J25" s="51"/>
@@ -3814,81 +3803,91 @@
       <c r="BK25" s="51"/>
       <c r="BL25" s="51"/>
     </row>
-    <row r="26" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="13"/>
-      <c r="B26" s="74" t="s">
-        <v>33</v>
-      </c>
-      <c r="C26" s="75"/>
-      <c r="D26" s="76"/>
-      <c r="E26" s="77"/>
-      <c r="F26" s="78"/>
+      <c r="B26" s="80" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" s="81" t="s">
+        <v>27</v>
+      </c>
+      <c r="D26" s="82">
+        <v>0</v>
+      </c>
+      <c r="E26" s="83">
+        <f>F23</f>
+        <v>45659</v>
+      </c>
+      <c r="F26" s="83">
+        <f>E26+14</f>
+        <v>45673</v>
+      </c>
       <c r="G26" s="17"/>
-      <c r="H26" s="5" t="str">
+      <c r="H26" s="5">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="I26" s="79"/>
-      <c r="J26" s="79"/>
-      <c r="K26" s="79"/>
-      <c r="L26" s="79"/>
-      <c r="M26" s="79"/>
-      <c r="N26" s="79"/>
-      <c r="O26" s="79"/>
-      <c r="P26" s="79"/>
-      <c r="Q26" s="79"/>
-      <c r="R26" s="79"/>
-      <c r="S26" s="79"/>
-      <c r="T26" s="79"/>
-      <c r="U26" s="79"/>
-      <c r="V26" s="79"/>
-      <c r="W26" s="79"/>
-      <c r="X26" s="79"/>
-      <c r="Y26" s="79"/>
-      <c r="Z26" s="79"/>
-      <c r="AA26" s="79"/>
-      <c r="AB26" s="79"/>
-      <c r="AC26" s="79"/>
-      <c r="AD26" s="79"/>
-      <c r="AE26" s="79"/>
-      <c r="AF26" s="79"/>
-      <c r="AG26" s="79"/>
-      <c r="AH26" s="79"/>
-      <c r="AI26" s="79"/>
-      <c r="AJ26" s="79"/>
-      <c r="AK26" s="79"/>
-      <c r="AL26" s="79"/>
-      <c r="AM26" s="79"/>
-      <c r="AN26" s="79"/>
-      <c r="AO26" s="79"/>
-      <c r="AP26" s="79"/>
-      <c r="AQ26" s="79"/>
-      <c r="AR26" s="79"/>
-      <c r="AS26" s="79"/>
-      <c r="AT26" s="79"/>
-      <c r="AU26" s="79"/>
-      <c r="AV26" s="79"/>
-      <c r="AW26" s="79"/>
-      <c r="AX26" s="79"/>
-      <c r="AY26" s="79"/>
-      <c r="AZ26" s="79"/>
-      <c r="BA26" s="79"/>
-      <c r="BB26" s="79"/>
-      <c r="BC26" s="79"/>
-      <c r="BD26" s="79"/>
-      <c r="BE26" s="79"/>
-      <c r="BF26" s="79"/>
-      <c r="BG26" s="79"/>
-      <c r="BH26" s="79"/>
-      <c r="BI26" s="79"/>
-      <c r="BJ26" s="79"/>
-      <c r="BK26" s="79"/>
-      <c r="BL26" s="79"/>
-    </row>
-    <row r="27" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="I26" s="51"/>
+      <c r="J26" s="51"/>
+      <c r="K26" s="51"/>
+      <c r="L26" s="51"/>
+      <c r="M26" s="51"/>
+      <c r="N26" s="51"/>
+      <c r="O26" s="51"/>
+      <c r="P26" s="51"/>
+      <c r="Q26" s="51"/>
+      <c r="R26" s="51"/>
+      <c r="S26" s="51"/>
+      <c r="T26" s="51"/>
+      <c r="U26" s="51"/>
+      <c r="V26" s="51"/>
+      <c r="W26" s="51"/>
+      <c r="X26" s="51"/>
+      <c r="Y26" s="51"/>
+      <c r="Z26" s="51"/>
+      <c r="AA26" s="51"/>
+      <c r="AB26" s="51"/>
+      <c r="AC26" s="51"/>
+      <c r="AD26" s="51"/>
+      <c r="AE26" s="51"/>
+      <c r="AF26" s="51"/>
+      <c r="AG26" s="51"/>
+      <c r="AH26" s="51"/>
+      <c r="AI26" s="51"/>
+      <c r="AJ26" s="51"/>
+      <c r="AK26" s="51"/>
+      <c r="AL26" s="51"/>
+      <c r="AM26" s="51"/>
+      <c r="AN26" s="51"/>
+      <c r="AO26" s="51"/>
+      <c r="AP26" s="51"/>
+      <c r="AQ26" s="51"/>
+      <c r="AR26" s="51"/>
+      <c r="AS26" s="51"/>
+      <c r="AT26" s="51"/>
+      <c r="AU26" s="51"/>
+      <c r="AV26" s="51"/>
+      <c r="AW26" s="51"/>
+      <c r="AX26" s="51"/>
+      <c r="AY26" s="51"/>
+      <c r="AZ26" s="51"/>
+      <c r="BA26" s="51"/>
+      <c r="BB26" s="51"/>
+      <c r="BC26" s="51"/>
+      <c r="BD26" s="51"/>
+      <c r="BE26" s="51"/>
+      <c r="BF26" s="51"/>
+      <c r="BG26" s="51"/>
+      <c r="BH26" s="51"/>
+      <c r="BI26" s="51"/>
+      <c r="BJ26" s="51"/>
+      <c r="BK26" s="51"/>
+      <c r="BL26" s="51"/>
+    </row>
+    <row r="27" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="13"/>
       <c r="B27" s="80" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C27" s="81" t="s">
         <v>27</v>
@@ -3897,12 +3896,12 @@
         <v>0</v>
       </c>
       <c r="E27" s="83">
-        <f xml:space="preserve"> F22</f>
-        <v>45613</v>
+        <f>F23</f>
+        <v>45659</v>
       </c>
       <c r="F27" s="83">
         <f>E27+14</f>
-        <v>45627</v>
+        <v>45673</v>
       </c>
       <c r="G27" s="17"/>
       <c r="H27" s="5">
@@ -3966,10 +3965,10 @@
       <c r="BK27" s="51"/>
       <c r="BL27" s="51"/>
     </row>
-    <row r="28" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="13"/>
       <c r="B28" s="80" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C28" s="81" t="s">
         <v>27</v>
@@ -3978,17 +3977,17 @@
         <v>0</v>
       </c>
       <c r="E28" s="83">
-        <f>F24</f>
+        <f>F23</f>
         <v>45659</v>
       </c>
       <c r="F28" s="83">
-        <f>E28+14</f>
-        <v>45673</v>
+        <f xml:space="preserve"> F27+21</f>
+        <v>45694</v>
       </c>
       <c r="G28" s="17"/>
       <c r="H28" s="5">
         <f t="shared" si="5"/>
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="I28" s="51"/>
       <c r="J28" s="51"/>
@@ -4047,10 +4046,10 @@
       <c r="BK28" s="51"/>
       <c r="BL28" s="51"/>
     </row>
-    <row r="29" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="13"/>
       <c r="B29" s="80" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C29" s="81" t="s">
         <v>27</v>
@@ -4059,17 +4058,16 @@
         <v>0</v>
       </c>
       <c r="E29" s="83">
-        <f>F24</f>
-        <v>45659</v>
-      </c>
-      <c r="F29" s="83">
-        <f>E29+14</f>
-        <v>45673</v>
+        <f xml:space="preserve"> F28</f>
+        <v>45694</v>
+      </c>
+      <c r="F29" s="83" t="s">
+        <v>48</v>
       </c>
       <c r="G29" s="17"/>
-      <c r="H29" s="5">
+      <c r="H29" s="5" t="e">
         <f t="shared" si="5"/>
-        <v>15</v>
+        <v>#VALUE!</v>
       </c>
       <c r="I29" s="51"/>
       <c r="J29" s="51"/>
@@ -4128,329 +4126,158 @@
       <c r="BK29" s="51"/>
       <c r="BL29" s="51"/>
     </row>
-    <row r="30" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="13"/>
-      <c r="B30" s="80" t="s">
-        <v>42</v>
-      </c>
-      <c r="C30" s="81" t="s">
-        <v>27</v>
-      </c>
-      <c r="D30" s="82">
-        <v>0</v>
-      </c>
-      <c r="E30" s="83">
-        <f>F24</f>
-        <v>45659</v>
-      </c>
-      <c r="F30" s="83">
-        <f xml:space="preserve"> F29+21</f>
-        <v>45694</v>
-      </c>
+      <c r="B30" s="84"/>
+      <c r="C30" s="85"/>
+      <c r="D30" s="86"/>
+      <c r="E30" s="87"/>
+      <c r="F30" s="87"/>
       <c r="G30" s="17"/>
-      <c r="H30" s="5">
-        <f t="shared" si="5"/>
-        <v>36</v>
-      </c>
-      <c r="I30" s="51"/>
-      <c r="J30" s="51"/>
-      <c r="K30" s="51"/>
-      <c r="L30" s="51"/>
-      <c r="M30" s="51"/>
-      <c r="N30" s="51"/>
-      <c r="O30" s="51"/>
-      <c r="P30" s="51"/>
-      <c r="Q30" s="51"/>
-      <c r="R30" s="51"/>
-      <c r="S30" s="51"/>
-      <c r="T30" s="51"/>
-      <c r="U30" s="51"/>
-      <c r="V30" s="51"/>
-      <c r="W30" s="51"/>
-      <c r="X30" s="51"/>
-      <c r="Y30" s="51"/>
-      <c r="Z30" s="51"/>
-      <c r="AA30" s="51"/>
-      <c r="AB30" s="51"/>
-      <c r="AC30" s="51"/>
-      <c r="AD30" s="51"/>
-      <c r="AE30" s="51"/>
-      <c r="AF30" s="51"/>
-      <c r="AG30" s="51"/>
-      <c r="AH30" s="51"/>
-      <c r="AI30" s="51"/>
-      <c r="AJ30" s="51"/>
-      <c r="AK30" s="51"/>
-      <c r="AL30" s="51"/>
-      <c r="AM30" s="51"/>
-      <c r="AN30" s="51"/>
-      <c r="AO30" s="51"/>
-      <c r="AP30" s="51"/>
-      <c r="AQ30" s="51"/>
-      <c r="AR30" s="51"/>
-      <c r="AS30" s="51"/>
-      <c r="AT30" s="51"/>
-      <c r="AU30" s="51"/>
-      <c r="AV30" s="51"/>
-      <c r="AW30" s="51"/>
-      <c r="AX30" s="51"/>
-      <c r="AY30" s="51"/>
-      <c r="AZ30" s="51"/>
-      <c r="BA30" s="51"/>
-      <c r="BB30" s="51"/>
-      <c r="BC30" s="51"/>
-      <c r="BD30" s="51"/>
-      <c r="BE30" s="51"/>
-      <c r="BF30" s="51"/>
-      <c r="BG30" s="51"/>
-      <c r="BH30" s="51"/>
-      <c r="BI30" s="51"/>
-      <c r="BJ30" s="51"/>
-      <c r="BK30" s="51"/>
-      <c r="BL30" s="51"/>
-    </row>
-    <row r="31" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="13"/>
-      <c r="B31" s="80" t="s">
-        <v>43</v>
-      </c>
-      <c r="C31" s="81" t="s">
-        <v>27</v>
-      </c>
-      <c r="D31" s="82">
-        <v>0</v>
-      </c>
-      <c r="E31" s="83">
-        <f xml:space="preserve"> F30</f>
-        <v>45694</v>
-      </c>
-      <c r="F31" s="83" t="s">
-        <v>49</v>
-      </c>
-      <c r="G31" s="17"/>
-      <c r="H31" s="5" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I31" s="51"/>
-      <c r="J31" s="51"/>
-      <c r="K31" s="51"/>
-      <c r="L31" s="51"/>
-      <c r="M31" s="51"/>
-      <c r="N31" s="51"/>
-      <c r="O31" s="51"/>
-      <c r="P31" s="51"/>
-      <c r="Q31" s="51"/>
-      <c r="R31" s="51"/>
-      <c r="S31" s="51"/>
-      <c r="T31" s="51"/>
-      <c r="U31" s="51"/>
-      <c r="V31" s="51"/>
-      <c r="W31" s="51"/>
-      <c r="X31" s="51"/>
-      <c r="Y31" s="51"/>
-      <c r="Z31" s="51"/>
-      <c r="AA31" s="51"/>
-      <c r="AB31" s="51"/>
-      <c r="AC31" s="51"/>
-      <c r="AD31" s="51"/>
-      <c r="AE31" s="51"/>
-      <c r="AF31" s="51"/>
-      <c r="AG31" s="51"/>
-      <c r="AH31" s="51"/>
-      <c r="AI31" s="51"/>
-      <c r="AJ31" s="51"/>
-      <c r="AK31" s="51"/>
-      <c r="AL31" s="51"/>
-      <c r="AM31" s="51"/>
-      <c r="AN31" s="51"/>
-      <c r="AO31" s="51"/>
-      <c r="AP31" s="51"/>
-      <c r="AQ31" s="51"/>
-      <c r="AR31" s="51"/>
-      <c r="AS31" s="51"/>
-      <c r="AT31" s="51"/>
-      <c r="AU31" s="51"/>
-      <c r="AV31" s="51"/>
-      <c r="AW31" s="51"/>
-      <c r="AX31" s="51"/>
-      <c r="AY31" s="51"/>
-      <c r="AZ31" s="51"/>
-      <c r="BA31" s="51"/>
-      <c r="BB31" s="51"/>
-      <c r="BC31" s="51"/>
-      <c r="BD31" s="51"/>
-      <c r="BE31" s="51"/>
-      <c r="BF31" s="51"/>
-      <c r="BG31" s="51"/>
-      <c r="BH31" s="51"/>
-      <c r="BI31" s="51"/>
-      <c r="BJ31" s="51"/>
-      <c r="BK31" s="51"/>
-      <c r="BL31" s="51"/>
-    </row>
-    <row r="32" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="13"/>
-      <c r="B32" s="84"/>
-      <c r="C32" s="85"/>
-      <c r="D32" s="86"/>
-      <c r="E32" s="87"/>
-      <c r="F32" s="87"/>
-      <c r="G32" s="17"/>
-      <c r="H32" s="5" t="str">
+      <c r="H30" s="5" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="I32" s="45"/>
-      <c r="J32" s="45"/>
-      <c r="K32" s="45"/>
-      <c r="L32" s="45"/>
-      <c r="M32" s="45"/>
-      <c r="N32" s="45"/>
-      <c r="O32" s="45"/>
-      <c r="P32" s="45"/>
-      <c r="Q32" s="45"/>
-      <c r="R32" s="45"/>
-      <c r="S32" s="45"/>
-      <c r="T32" s="45"/>
-      <c r="U32" s="45"/>
-      <c r="V32" s="45"/>
-      <c r="W32" s="45"/>
-      <c r="X32" s="45"/>
-      <c r="Y32" s="45"/>
-      <c r="Z32" s="45"/>
-      <c r="AA32" s="45"/>
-      <c r="AB32" s="45"/>
-      <c r="AC32" s="45"/>
-      <c r="AD32" s="45"/>
-      <c r="AE32" s="45"/>
-      <c r="AF32" s="45"/>
-      <c r="AG32" s="45"/>
-      <c r="AH32" s="45"/>
-      <c r="AI32" s="45"/>
-      <c r="AJ32" s="45"/>
-      <c r="AK32" s="45"/>
-      <c r="AL32" s="45"/>
-      <c r="AM32" s="45"/>
-      <c r="AN32" s="45"/>
-      <c r="AO32" s="45"/>
-      <c r="AP32" s="45"/>
-      <c r="AQ32" s="45"/>
-      <c r="AR32" s="45"/>
-      <c r="AS32" s="45"/>
-      <c r="AT32" s="45"/>
-      <c r="AU32" s="45"/>
-      <c r="AV32" s="45"/>
-      <c r="AW32" s="45"/>
-      <c r="AX32" s="45"/>
-      <c r="AY32" s="45"/>
-      <c r="AZ32" s="45"/>
-      <c r="BA32" s="45"/>
-      <c r="BB32" s="45"/>
-      <c r="BC32" s="45"/>
-      <c r="BD32" s="45"/>
-      <c r="BE32" s="45"/>
-      <c r="BF32" s="45"/>
-      <c r="BG32" s="45"/>
-      <c r="BH32" s="45"/>
-      <c r="BI32" s="45"/>
-      <c r="BJ32" s="45"/>
-      <c r="BK32" s="45"/>
-      <c r="BL32" s="45"/>
-    </row>
-    <row r="33" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="14"/>
-      <c r="B33" s="88" t="s">
+      <c r="I30" s="45"/>
+      <c r="J30" s="45"/>
+      <c r="K30" s="45"/>
+      <c r="L30" s="45"/>
+      <c r="M30" s="45"/>
+      <c r="N30" s="45"/>
+      <c r="O30" s="45"/>
+      <c r="P30" s="45"/>
+      <c r="Q30" s="45"/>
+      <c r="R30" s="45"/>
+      <c r="S30" s="45"/>
+      <c r="T30" s="45"/>
+      <c r="U30" s="45"/>
+      <c r="V30" s="45"/>
+      <c r="W30" s="45"/>
+      <c r="X30" s="45"/>
+      <c r="Y30" s="45"/>
+      <c r="Z30" s="45"/>
+      <c r="AA30" s="45"/>
+      <c r="AB30" s="45"/>
+      <c r="AC30" s="45"/>
+      <c r="AD30" s="45"/>
+      <c r="AE30" s="45"/>
+      <c r="AF30" s="45"/>
+      <c r="AG30" s="45"/>
+      <c r="AH30" s="45"/>
+      <c r="AI30" s="45"/>
+      <c r="AJ30" s="45"/>
+      <c r="AK30" s="45"/>
+      <c r="AL30" s="45"/>
+      <c r="AM30" s="45"/>
+      <c r="AN30" s="45"/>
+      <c r="AO30" s="45"/>
+      <c r="AP30" s="45"/>
+      <c r="AQ30" s="45"/>
+      <c r="AR30" s="45"/>
+      <c r="AS30" s="45"/>
+      <c r="AT30" s="45"/>
+      <c r="AU30" s="45"/>
+      <c r="AV30" s="45"/>
+      <c r="AW30" s="45"/>
+      <c r="AX30" s="45"/>
+      <c r="AY30" s="45"/>
+      <c r="AZ30" s="45"/>
+      <c r="BA30" s="45"/>
+      <c r="BB30" s="45"/>
+      <c r="BC30" s="45"/>
+      <c r="BD30" s="45"/>
+      <c r="BE30" s="45"/>
+      <c r="BF30" s="45"/>
+      <c r="BG30" s="45"/>
+      <c r="BH30" s="45"/>
+      <c r="BI30" s="45"/>
+      <c r="BJ30" s="45"/>
+      <c r="BK30" s="45"/>
+      <c r="BL30" s="45"/>
+    </row>
+    <row r="31" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="14"/>
+      <c r="B31" s="88" t="s">
         <v>0</v>
       </c>
-      <c r="C33" s="89"/>
-      <c r="D33" s="90"/>
-      <c r="E33" s="91"/>
-      <c r="F33" s="92"/>
-      <c r="G33" s="17"/>
-      <c r="H33" s="6" t="str">
+      <c r="C31" s="89"/>
+      <c r="D31" s="90"/>
+      <c r="E31" s="91"/>
+      <c r="F31" s="92"/>
+      <c r="G31" s="17"/>
+      <c r="H31" s="6" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="I33" s="93"/>
-      <c r="J33" s="93"/>
-      <c r="K33" s="93"/>
-      <c r="L33" s="93"/>
-      <c r="M33" s="93"/>
-      <c r="N33" s="93"/>
-      <c r="O33" s="93"/>
-      <c r="P33" s="93"/>
-      <c r="Q33" s="93"/>
-      <c r="R33" s="93"/>
-      <c r="S33" s="93"/>
-      <c r="T33" s="93"/>
-      <c r="U33" s="93"/>
-      <c r="V33" s="93"/>
-      <c r="W33" s="93"/>
-      <c r="X33" s="93"/>
-      <c r="Y33" s="93"/>
-      <c r="Z33" s="93"/>
-      <c r="AA33" s="93"/>
-      <c r="AB33" s="93"/>
-      <c r="AC33" s="93"/>
-      <c r="AD33" s="93"/>
-      <c r="AE33" s="93"/>
-      <c r="AF33" s="93"/>
-      <c r="AG33" s="93"/>
-      <c r="AH33" s="93"/>
-      <c r="AI33" s="93"/>
-      <c r="AJ33" s="93"/>
-      <c r="AK33" s="93"/>
-      <c r="AL33" s="93"/>
-      <c r="AM33" s="93"/>
-      <c r="AN33" s="93"/>
-      <c r="AO33" s="93"/>
-      <c r="AP33" s="93"/>
-      <c r="AQ33" s="93"/>
-      <c r="AR33" s="93"/>
-      <c r="AS33" s="93"/>
-      <c r="AT33" s="93"/>
-      <c r="AU33" s="93"/>
-      <c r="AV33" s="93"/>
-      <c r="AW33" s="93"/>
-      <c r="AX33" s="93"/>
-      <c r="AY33" s="93"/>
-      <c r="AZ33" s="93"/>
-      <c r="BA33" s="93"/>
-      <c r="BB33" s="93"/>
-      <c r="BC33" s="93"/>
-      <c r="BD33" s="93"/>
-      <c r="BE33" s="93"/>
-      <c r="BF33" s="93"/>
-      <c r="BG33" s="93"/>
-      <c r="BH33" s="93"/>
-      <c r="BI33" s="93"/>
-      <c r="BJ33" s="93"/>
-      <c r="BK33" s="93"/>
-      <c r="BL33" s="93"/>
-    </row>
-    <row r="34" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G34" s="3"/>
-    </row>
-    <row r="35" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C35" s="16"/>
-      <c r="F35" s="15"/>
-    </row>
-    <row r="36" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C36" s="4"/>
+      <c r="I31" s="93"/>
+      <c r="J31" s="93"/>
+      <c r="K31" s="93"/>
+      <c r="L31" s="93"/>
+      <c r="M31" s="93"/>
+      <c r="N31" s="93"/>
+      <c r="O31" s="93"/>
+      <c r="P31" s="93"/>
+      <c r="Q31" s="93"/>
+      <c r="R31" s="93"/>
+      <c r="S31" s="93"/>
+      <c r="T31" s="93"/>
+      <c r="U31" s="93"/>
+      <c r="V31" s="93"/>
+      <c r="W31" s="93"/>
+      <c r="X31" s="93"/>
+      <c r="Y31" s="93"/>
+      <c r="Z31" s="93"/>
+      <c r="AA31" s="93"/>
+      <c r="AB31" s="93"/>
+      <c r="AC31" s="93"/>
+      <c r="AD31" s="93"/>
+      <c r="AE31" s="93"/>
+      <c r="AF31" s="93"/>
+      <c r="AG31" s="93"/>
+      <c r="AH31" s="93"/>
+      <c r="AI31" s="93"/>
+      <c r="AJ31" s="93"/>
+      <c r="AK31" s="93"/>
+      <c r="AL31" s="93"/>
+      <c r="AM31" s="93"/>
+      <c r="AN31" s="93"/>
+      <c r="AO31" s="93"/>
+      <c r="AP31" s="93"/>
+      <c r="AQ31" s="93"/>
+      <c r="AR31" s="93"/>
+      <c r="AS31" s="93"/>
+      <c r="AT31" s="93"/>
+      <c r="AU31" s="93"/>
+      <c r="AV31" s="93"/>
+      <c r="AW31" s="93"/>
+      <c r="AX31" s="93"/>
+      <c r="AY31" s="93"/>
+      <c r="AZ31" s="93"/>
+      <c r="BA31" s="93"/>
+      <c r="BB31" s="93"/>
+      <c r="BC31" s="93"/>
+      <c r="BD31" s="93"/>
+      <c r="BE31" s="93"/>
+      <c r="BF31" s="93"/>
+      <c r="BG31" s="93"/>
+      <c r="BH31" s="93"/>
+      <c r="BI31" s="93"/>
+      <c r="BJ31" s="93"/>
+      <c r="BK31" s="93"/>
+      <c r="BL31" s="93"/>
+    </row>
+    <row r="32" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G32" s="3"/>
+    </row>
+    <row r="33" spans="3:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C33" s="16"/>
+      <c r="F33" s="15"/>
+    </row>
+    <row r="34" spans="3:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C34" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="Q2:Z2"/>
-    <mergeCell ref="Q1:Z1"/>
-    <mergeCell ref="I1:O1"/>
-    <mergeCell ref="I2:O2"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="I4:O4"/>
     <mergeCell ref="P4:V4"/>
@@ -4459,8 +4286,18 @@
     <mergeCell ref="AK4:AQ4"/>
     <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="Q2:Z2"/>
+    <mergeCell ref="Q1:Z1"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="I2:O2"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
   </mergeCells>
-  <conditionalFormatting sqref="D7:D33">
+  <conditionalFormatting sqref="D7:D31">
     <cfRule type="dataBar" priority="23">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -4474,7 +4311,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I4:BL31">
+  <conditionalFormatting sqref="I4:BL29">
     <cfRule type="expression" dxfId="8" priority="1">
       <formula>AND(TODAY()&gt;=I$5, TODAY()&lt;J$5)</formula>
     </cfRule>
@@ -4487,7 +4324,7 @@
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I15:BL19">
+  <conditionalFormatting sqref="I15:BL18">
     <cfRule type="expression" dxfId="5" priority="4">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
@@ -4495,7 +4332,7 @@
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I21:BL25">
+  <conditionalFormatting sqref="I20:BL23">
     <cfRule type="expression" dxfId="3" priority="2">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
@@ -4503,7 +4340,7 @@
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I27:BL31">
+  <conditionalFormatting sqref="I25:BL29">
     <cfRule type="expression" dxfId="1" priority="36">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
@@ -4524,9 +4361,9 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="B9 contains the task name.  C9 is the assignee.  D9 is a progress bar that shades based on the number entered into the cell.  _x000a__x000a_E9 contains the start date and F9 contains the end date._x000a__x000a_The Gantt chart will fill in starting in cell I9 based on task dates." sqref="A9" xr:uid="{D870A2F6-6B07-4F5A-A81D-4BCCFADF8796}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Rows 10 through 13 repeat the pattern from row 9. _x000a__x000a_Repeat the instructions from cell A9 for all task rows in this worksheet. _x000a__x000a_Continue entering tasks in cells A10 through A13 or go to cell A14 to learn more." sqref="A10" xr:uid="{872449A7-C3CC-45B6-BA90-B1AAD66BA0E5}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Cell B14 contains the Phase 2 sample title. Enter a new title in cell B14._x000a_To delete the phase and work only from tasks, simply delete this row. To remove the phase, simply delete the row. Add tasks to previous phase by entering a new row above this one._x000a_" sqref="A14" xr:uid="{4F48FC41-E335-47F1-87AA-3333A52AD81C}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Phase 3's sample block starts in cell B20." sqref="A20" xr:uid="{956902D1-D3B5-416D-BB69-9362D193BC0A}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Phase 4's sample block starts in cell B26." sqref="A26" xr:uid="{DE54E5DE-526D-4D71-8D03-E99B4AB2FEE5}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This row marks the end of the Project Schedule. DO NOT enter anything in this row. _x000a_Insert new rows ABOVE this one to continue building out your Project Schedule." sqref="A33" xr:uid="{79B9237E-4DD3-4E0F-8ED6-E0B695A99D96}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Phase 3's sample block starts in cell B20." sqref="A19" xr:uid="{956902D1-D3B5-416D-BB69-9362D193BC0A}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Phase 4's sample block starts in cell B26." sqref="A24" xr:uid="{DE54E5DE-526D-4D71-8D03-E99B4AB2FEE5}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This row marks the end of the Project Schedule. DO NOT enter anything in this row. _x000a_Insert new rows ABOVE this one to continue building out your Project Schedule." sqref="A31" xr:uid="{79B9237E-4DD3-4E0F-8ED6-E0B695A99D96}"/>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -4534,7 +4371,7 @@
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.35" right="0.35" top="0.35" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup scale="57" fitToHeight="0" orientation="landscape" r:id="rId3"/>
+  <pageSetup scale="49" fitToHeight="0" orientation="landscape" r:id="rId3"/>
   <headerFooter differentFirst="1" scaleWithDoc="0">
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
@@ -4554,7 +4391,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D7:D33</xm:sqref>
+          <xm:sqref>D7:D31</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -4566,112 +4403,112 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="87" style="7" customWidth="1"/>
     <col min="2" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="1:2" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:2" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A2" s="97" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="8"/>
     </row>
-    <row r="3" spans="1:2" s="11" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" s="11" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="98"/>
       <c r="B3" s="12"/>
     </row>
-    <row r="4" spans="1:2" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:2" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.7">
       <c r="A4" s="99" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="100" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="99" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:2" s="7" customFormat="1" ht="205.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" s="7" customFormat="1" ht="205.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="101" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:2" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.6">
+    <row r="8" spans="1:2" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.7">
       <c r="A8" s="99" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="57" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A9" s="100" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2" s="7" customFormat="1" ht="28.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" s="7" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="102" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:2" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.6">
+    <row r="11" spans="1:2" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.7">
       <c r="A11" s="99" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A12" s="100" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:2" s="7" customFormat="1" ht="28.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" s="7" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="102" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:2" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.6">
+    <row r="14" spans="1:2" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.7">
       <c r="A14" s="99" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="100" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" ht="69" x14ac:dyDescent="0.25">
       <c r="A16" s="100" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="103"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="103"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="103"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="103"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="103"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="103"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="103"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="103"/>
     </row>
   </sheetData>
@@ -4687,23 +4524,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5019,29 +4845,29 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A82239A0-E68C-493F-BEE6-C77FEA397FD6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5068,9 +4894,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A82239A0-E68C-493F-BEE6-C77FEA397FD6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
normalized input and removed y coordinate
</commit_message>
<xml_diff>
--- a/project plan.xlsx
+++ b/project plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\augus\Desktop\MainFolder\University\Master\MscThesis\Project\Git\AI_Lora_Mobility\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADF95A60-90E6-45F9-869F-615FB87CC8FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BFEF3C7-68AA-42EB-A759-123A3649558B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1085,19 +1085,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="167" fontId="19" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="19" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="19" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1109,17 +1112,14 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="167" fontId="19" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="19" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="19" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1721,8 +1721,8 @@
   </sheetPr>
   <dimension ref="A1:BL34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1748,28 +1748,28 @@
       <c r="E1" s="20"/>
       <c r="F1" s="21"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="112" t="s">
+      <c r="I1" s="113" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="113"/>
-      <c r="K1" s="113"/>
-      <c r="L1" s="113"/>
-      <c r="M1" s="113"/>
-      <c r="N1" s="113"/>
-      <c r="O1" s="113"/>
+      <c r="J1" s="114"/>
+      <c r="K1" s="114"/>
+      <c r="L1" s="114"/>
+      <c r="M1" s="114"/>
+      <c r="N1" s="114"/>
+      <c r="O1" s="114"/>
       <c r="P1" s="24"/>
-      <c r="Q1" s="111">
+      <c r="Q1" s="112">
         <v>45537</v>
       </c>
-      <c r="R1" s="110"/>
-      <c r="S1" s="110"/>
-      <c r="T1" s="110"/>
-      <c r="U1" s="110"/>
-      <c r="V1" s="110"/>
-      <c r="W1" s="110"/>
-      <c r="X1" s="110"/>
-      <c r="Y1" s="110"/>
-      <c r="Z1" s="110"/>
+      <c r="R1" s="111"/>
+      <c r="S1" s="111"/>
+      <c r="T1" s="111"/>
+      <c r="U1" s="111"/>
+      <c r="V1" s="111"/>
+      <c r="W1" s="111"/>
+      <c r="X1" s="111"/>
+      <c r="Y1" s="111"/>
+      <c r="Z1" s="111"/>
     </row>
     <row r="2" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B2" s="94" t="s">
@@ -1781,28 +1781,28 @@
       <c r="D2" s="22"/>
       <c r="E2" s="23"/>
       <c r="F2" s="22"/>
-      <c r="I2" s="112" t="s">
+      <c r="I2" s="113" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="113"/>
-      <c r="K2" s="113"/>
-      <c r="L2" s="113"/>
-      <c r="M2" s="113"/>
-      <c r="N2" s="113"/>
-      <c r="O2" s="113"/>
+      <c r="J2" s="114"/>
+      <c r="K2" s="114"/>
+      <c r="L2" s="114"/>
+      <c r="M2" s="114"/>
+      <c r="N2" s="114"/>
+      <c r="O2" s="114"/>
       <c r="P2" s="24"/>
-      <c r="Q2" s="109">
+      <c r="Q2" s="110">
         <v>7</v>
       </c>
-      <c r="R2" s="110"/>
-      <c r="S2" s="110"/>
-      <c r="T2" s="110"/>
-      <c r="U2" s="110"/>
-      <c r="V2" s="110"/>
-      <c r="W2" s="110"/>
-      <c r="X2" s="110"/>
-      <c r="Y2" s="110"/>
-      <c r="Z2" s="110"/>
+      <c r="R2" s="111"/>
+      <c r="S2" s="111"/>
+      <c r="T2" s="111"/>
+      <c r="U2" s="111"/>
+      <c r="V2" s="111"/>
+      <c r="W2" s="111"/>
+      <c r="X2" s="111"/>
+      <c r="Y2" s="111"/>
+      <c r="Z2" s="111"/>
     </row>
     <row r="3" spans="1:64" s="26" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
@@ -1818,102 +1818,102 @@
         <v>13</v>
       </c>
       <c r="E4" s="30"/>
-      <c r="I4" s="106">
+      <c r="I4" s="117">
         <f>I5</f>
         <v>45579</v>
       </c>
-      <c r="J4" s="104"/>
-      <c r="K4" s="104"/>
-      <c r="L4" s="104"/>
-      <c r="M4" s="104"/>
-      <c r="N4" s="104"/>
-      <c r="O4" s="104"/>
-      <c r="P4" s="104">
+      <c r="J4" s="115"/>
+      <c r="K4" s="115"/>
+      <c r="L4" s="115"/>
+      <c r="M4" s="115"/>
+      <c r="N4" s="115"/>
+      <c r="O4" s="115"/>
+      <c r="P4" s="115">
         <f>P5</f>
         <v>45586</v>
       </c>
-      <c r="Q4" s="104"/>
-      <c r="R4" s="104"/>
-      <c r="S4" s="104"/>
-      <c r="T4" s="104"/>
-      <c r="U4" s="104"/>
-      <c r="V4" s="104"/>
-      <c r="W4" s="104">
+      <c r="Q4" s="115"/>
+      <c r="R4" s="115"/>
+      <c r="S4" s="115"/>
+      <c r="T4" s="115"/>
+      <c r="U4" s="115"/>
+      <c r="V4" s="115"/>
+      <c r="W4" s="115">
         <f>W5</f>
         <v>45593</v>
       </c>
-      <c r="X4" s="104"/>
-      <c r="Y4" s="104"/>
-      <c r="Z4" s="104"/>
-      <c r="AA4" s="104"/>
-      <c r="AB4" s="104"/>
-      <c r="AC4" s="104"/>
-      <c r="AD4" s="104">
+      <c r="X4" s="115"/>
+      <c r="Y4" s="115"/>
+      <c r="Z4" s="115"/>
+      <c r="AA4" s="115"/>
+      <c r="AB4" s="115"/>
+      <c r="AC4" s="115"/>
+      <c r="AD4" s="115">
         <f>AD5</f>
         <v>45600</v>
       </c>
-      <c r="AE4" s="104"/>
-      <c r="AF4" s="104"/>
-      <c r="AG4" s="104"/>
-      <c r="AH4" s="104"/>
-      <c r="AI4" s="104"/>
-      <c r="AJ4" s="104"/>
-      <c r="AK4" s="104">
+      <c r="AE4" s="115"/>
+      <c r="AF4" s="115"/>
+      <c r="AG4" s="115"/>
+      <c r="AH4" s="115"/>
+      <c r="AI4" s="115"/>
+      <c r="AJ4" s="115"/>
+      <c r="AK4" s="115">
         <f>AK5</f>
         <v>45607</v>
       </c>
-      <c r="AL4" s="104"/>
-      <c r="AM4" s="104"/>
-      <c r="AN4" s="104"/>
-      <c r="AO4" s="104"/>
-      <c r="AP4" s="104"/>
-      <c r="AQ4" s="104"/>
-      <c r="AR4" s="104">
+      <c r="AL4" s="115"/>
+      <c r="AM4" s="115"/>
+      <c r="AN4" s="115"/>
+      <c r="AO4" s="115"/>
+      <c r="AP4" s="115"/>
+      <c r="AQ4" s="115"/>
+      <c r="AR4" s="115">
         <f>AR5</f>
         <v>45614</v>
       </c>
-      <c r="AS4" s="104"/>
-      <c r="AT4" s="104"/>
-      <c r="AU4" s="104"/>
-      <c r="AV4" s="104"/>
-      <c r="AW4" s="104"/>
-      <c r="AX4" s="104"/>
-      <c r="AY4" s="104">
+      <c r="AS4" s="115"/>
+      <c r="AT4" s="115"/>
+      <c r="AU4" s="115"/>
+      <c r="AV4" s="115"/>
+      <c r="AW4" s="115"/>
+      <c r="AX4" s="115"/>
+      <c r="AY4" s="115">
         <f>AY5</f>
         <v>45621</v>
       </c>
-      <c r="AZ4" s="104"/>
-      <c r="BA4" s="104"/>
-      <c r="BB4" s="104"/>
-      <c r="BC4" s="104"/>
-      <c r="BD4" s="104"/>
-      <c r="BE4" s="104"/>
-      <c r="BF4" s="104">
+      <c r="AZ4" s="115"/>
+      <c r="BA4" s="115"/>
+      <c r="BB4" s="115"/>
+      <c r="BC4" s="115"/>
+      <c r="BD4" s="115"/>
+      <c r="BE4" s="115"/>
+      <c r="BF4" s="115">
         <f>BF5</f>
         <v>45628</v>
       </c>
-      <c r="BG4" s="104"/>
-      <c r="BH4" s="104"/>
-      <c r="BI4" s="104"/>
-      <c r="BJ4" s="104"/>
-      <c r="BK4" s="104"/>
-      <c r="BL4" s="105"/>
+      <c r="BG4" s="115"/>
+      <c r="BH4" s="115"/>
+      <c r="BI4" s="115"/>
+      <c r="BJ4" s="115"/>
+      <c r="BK4" s="115"/>
+      <c r="BL4" s="116"/>
     </row>
     <row r="5" spans="1:64" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="114"/>
-      <c r="B5" s="115" t="s">
+      <c r="A5" s="104"/>
+      <c r="B5" s="105" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="117" t="s">
+      <c r="C5" s="107" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="107" t="s">
+      <c r="D5" s="109" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="107" t="s">
+      <c r="E5" s="109" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="107" t="s">
+      <c r="F5" s="109" t="s">
         <v>4</v>
       </c>
       <c r="I5" s="31">
@@ -2142,8 +2142,8 @@
       </c>
     </row>
     <row r="6" spans="1:64" s="26" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="114"/>
-      <c r="B6" s="116"/>
+      <c r="A6" s="104"/>
+      <c r="B6" s="106"/>
       <c r="C6" s="108"/>
       <c r="D6" s="108"/>
       <c r="E6" s="108"/>
@@ -2603,7 +2603,7 @@
         <v>27</v>
       </c>
       <c r="D10" s="49">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="E10" s="53">
         <f>E9</f>
@@ -2684,7 +2684,7 @@
         <v>27</v>
       </c>
       <c r="D11" s="49">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="E11" s="53">
         <v>45550</v>
@@ -2764,7 +2764,7 @@
         <v>27</v>
       </c>
       <c r="D12" s="49">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="E12" s="53">
         <f>F10-7</f>
@@ -2845,7 +2845,7 @@
         <v>27</v>
       </c>
       <c r="D13" s="49">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="E13" s="53">
         <f xml:space="preserve"> E11</f>
@@ -2941,7 +2941,7 @@
         <v>27</v>
       </c>
       <c r="D15" s="62">
-        <v>0.1</v>
+        <v>0.99</v>
       </c>
       <c r="E15" s="63">
         <f>F12</f>
@@ -3336,7 +3336,7 @@
         <v>27</v>
       </c>
       <c r="D20" s="72">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="E20" s="73">
         <f xml:space="preserve"> F18</f>
@@ -3417,7 +3417,7 @@
         <v>27</v>
       </c>
       <c r="D21" s="72">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="E21" s="73">
         <f xml:space="preserve"> F18</f>
@@ -4278,16 +4278,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="Q2:Z2"/>
-    <mergeCell ref="Q1:Z1"/>
-    <mergeCell ref="I1:O1"/>
-    <mergeCell ref="I2:O2"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="I4:O4"/>
     <mergeCell ref="P4:V4"/>
@@ -4296,6 +4286,16 @@
     <mergeCell ref="AK4:AQ4"/>
     <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="Q2:Z2"/>
+    <mergeCell ref="Q1:Z1"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="I2:O2"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D31">
     <cfRule type="dataBar" priority="23">
@@ -4524,23 +4524,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4856,29 +4845,29 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A82239A0-E68C-493F-BEE6-C77FEA397FD6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4905,9 +4894,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A82239A0-E68C-493F-BEE6-C77FEA397FD6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>